<commit_message>
- Typo: Cacge -> Cache (fixed #680)
</commit_message>
<xml_diff>
--- a/Language/Resources.xlsx
+++ b/Language/Resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pasta\Documents\Visual Studio 2017\Projects\NeeView\Language\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70575E9-1CF2-4E37-92DF-10DA5C2315E4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3035D31-D8F6-4C5C-965F-A4A98E4ABAE5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="3525" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11829,9 +11829,6 @@
   </si>
   <si>
     <t>SettingPageVisualThumbnailCache</t>
-  </si>
-  <si>
-    <t>Cacge</t>
   </si>
   <si>
     <t>キャッシュ</t>
@@ -12468,6 +12465,10 @@
   </si>
   <si>
     <t>0を指定すると画面がちらつくことがあります。</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Cache</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -12837,8 +12838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1537"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1202" workbookViewId="0">
-      <selection activeCell="B1218" sqref="B1218"/>
+    <sheetView tabSelected="1" topLeftCell="B1441" workbookViewId="0">
+      <selection activeCell="B1444" sqref="B1444"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -26235,21 +26236,21 @@
         <v>3345</v>
       </c>
       <c r="B1217" s="1" t="s">
-        <v>4120</v>
+        <v>4119</v>
       </c>
       <c r="C1217" s="1" t="s">
-        <v>4122</v>
+        <v>4121</v>
       </c>
     </row>
     <row r="1218" spans="1:3">
       <c r="A1218" s="1" t="s">
-        <v>4119</v>
+        <v>4118</v>
       </c>
       <c r="B1218" s="1" t="s">
-        <v>4121</v>
+        <v>4120</v>
       </c>
       <c r="C1218" s="1" t="s">
-        <v>4123</v>
+        <v>4122</v>
       </c>
     </row>
     <row r="1219" spans="1:3">
@@ -28864,51 +28865,51 @@
         <v>3920</v>
       </c>
       <c r="B1456" s="1" t="s">
+        <v>4123</v>
+      </c>
+      <c r="C1456" s="1" t="s">
         <v>3921</v>
-      </c>
-      <c r="C1456" s="1" t="s">
-        <v>3922</v>
       </c>
     </row>
     <row r="1457" spans="1:3">
       <c r="A1457" s="1" t="s">
+        <v>3922</v>
+      </c>
+      <c r="B1457" s="1" t="s">
         <v>3923</v>
       </c>
-      <c r="B1457" s="1" t="s">
+      <c r="C1457" s="1" t="s">
         <v>3924</v>
-      </c>
-      <c r="C1457" s="1" t="s">
-        <v>3925</v>
       </c>
     </row>
     <row r="1458" spans="1:3">
       <c r="A1458" s="1" t="s">
+        <v>3925</v>
+      </c>
+      <c r="B1458" s="1" t="s">
         <v>3926</v>
       </c>
-      <c r="B1458" s="1" t="s">
+      <c r="C1458" s="1" t="s">
         <v>3927</v>
-      </c>
-      <c r="C1458" s="1" t="s">
-        <v>3928</v>
       </c>
     </row>
     <row r="1459" spans="1:3">
       <c r="A1459" s="1" t="s">
+        <v>3928</v>
+      </c>
+      <c r="B1459" s="1" t="s">
         <v>3929</v>
       </c>
-      <c r="B1459" s="1" t="s">
+      <c r="C1459" s="1" t="s">
         <v>3930</v>
-      </c>
-      <c r="C1459" s="1" t="s">
-        <v>3931</v>
       </c>
     </row>
     <row r="1460" spans="1:3">
       <c r="A1460" s="1" t="s">
+        <v>3931</v>
+      </c>
+      <c r="B1460" s="1" t="s">
         <v>3932</v>
-      </c>
-      <c r="B1460" s="1" t="s">
-        <v>3933</v>
       </c>
       <c r="C1460" s="1" t="s">
         <v>1480</v>
@@ -28916,62 +28917,62 @@
     </row>
     <row r="1461" spans="1:3" ht="281.25">
       <c r="A1461" s="1" t="s">
+        <v>3933</v>
+      </c>
+      <c r="B1461" s="3" t="s">
         <v>3934</v>
       </c>
-      <c r="B1461" s="3" t="s">
+      <c r="C1461" s="3" t="s">
         <v>3935</v>
-      </c>
-      <c r="C1461" s="3" t="s">
-        <v>3936</v>
       </c>
     </row>
     <row r="1462" spans="1:3">
       <c r="A1462" s="1" t="s">
+        <v>3936</v>
+      </c>
+      <c r="B1462" s="1" t="s">
         <v>3937</v>
       </c>
-      <c r="B1462" s="1" t="s">
+      <c r="C1462" s="1" t="s">
         <v>3938</v>
-      </c>
-      <c r="C1462" s="1" t="s">
-        <v>3939</v>
       </c>
     </row>
     <row r="1463" spans="1:3">
       <c r="A1463" s="1" t="s">
+        <v>3939</v>
+      </c>
+      <c r="B1463" s="1" t="s">
         <v>3940</v>
       </c>
-      <c r="B1463" s="1" t="s">
+      <c r="C1463" s="1" t="s">
         <v>3941</v>
-      </c>
-      <c r="C1463" s="1" t="s">
-        <v>3942</v>
       </c>
     </row>
     <row r="1464" spans="1:3" ht="37.5">
       <c r="A1464" s="1" t="s">
+        <v>3942</v>
+      </c>
+      <c r="B1464" s="3" t="s">
         <v>3943</v>
       </c>
-      <c r="B1464" s="3" t="s">
+      <c r="C1464" s="3" t="s">
         <v>3944</v>
-      </c>
-      <c r="C1464" s="3" t="s">
-        <v>3945</v>
       </c>
     </row>
     <row r="1465" spans="1:3">
       <c r="A1465" s="1" t="s">
+        <v>3945</v>
+      </c>
+      <c r="B1465" s="1" t="s">
         <v>3946</v>
       </c>
-      <c r="B1465" s="1" t="s">
+      <c r="C1465" s="1" t="s">
         <v>3947</v>
-      </c>
-      <c r="C1465" s="1" t="s">
-        <v>3948</v>
       </c>
     </row>
     <row r="1466" spans="1:3">
       <c r="A1466" s="1" t="s">
-        <v>3949</v>
+        <v>3948</v>
       </c>
       <c r="B1466" s="1" t="s">
         <v>1627</v>
@@ -28982,29 +28983,29 @@
     </row>
     <row r="1467" spans="1:3">
       <c r="A1467" s="1" t="s">
+        <v>3949</v>
+      </c>
+      <c r="B1467" s="1" t="s">
         <v>3950</v>
       </c>
-      <c r="B1467" s="1" t="s">
+      <c r="C1467" s="1" t="s">
         <v>3951</v>
-      </c>
-      <c r="C1467" s="1" t="s">
-        <v>3952</v>
       </c>
     </row>
     <row r="1468" spans="1:3">
       <c r="A1468" s="1" t="s">
+        <v>3952</v>
+      </c>
+      <c r="B1468" s="1" t="s">
         <v>3953</v>
       </c>
-      <c r="B1468" s="1" t="s">
+      <c r="C1468" s="1" t="s">
         <v>3954</v>
-      </c>
-      <c r="C1468" s="1" t="s">
-        <v>3955</v>
       </c>
     </row>
     <row r="1469" spans="1:3">
       <c r="A1469" s="1" t="s">
-        <v>3956</v>
+        <v>3955</v>
       </c>
       <c r="B1469" s="1" t="s">
         <v>44</v>
@@ -29015,7 +29016,7 @@
     </row>
     <row r="1470" spans="1:3">
       <c r="A1470" s="1" t="s">
-        <v>3957</v>
+        <v>3956</v>
       </c>
       <c r="B1470" s="1" t="s">
         <v>98</v>
@@ -29026,51 +29027,51 @@
     </row>
     <row r="1471" spans="1:3">
       <c r="A1471" s="1" t="s">
+        <v>3957</v>
+      </c>
+      <c r="B1471" s="1" t="s">
         <v>3958</v>
       </c>
-      <c r="B1471" s="1" t="s">
+      <c r="C1471" s="1" t="s">
         <v>3959</v>
-      </c>
-      <c r="C1471" s="1" t="s">
-        <v>3960</v>
       </c>
     </row>
     <row r="1472" spans="1:3">
       <c r="A1472" s="1" t="s">
+        <v>3960</v>
+      </c>
+      <c r="B1472" s="1" t="s">
         <v>3961</v>
       </c>
-      <c r="B1472" s="1" t="s">
+      <c r="C1472" s="1" t="s">
         <v>3962</v>
-      </c>
-      <c r="C1472" s="1" t="s">
-        <v>3963</v>
       </c>
     </row>
     <row r="1473" spans="1:3">
       <c r="A1473" s="1" t="s">
+        <v>3963</v>
+      </c>
+      <c r="B1473" s="1" t="s">
         <v>3964</v>
       </c>
-      <c r="B1473" s="1" t="s">
+      <c r="C1473" s="1" t="s">
         <v>3965</v>
-      </c>
-      <c r="C1473" s="1" t="s">
-        <v>3966</v>
       </c>
     </row>
     <row r="1474" spans="1:3">
       <c r="A1474" s="1" t="s">
+        <v>3966</v>
+      </c>
+      <c r="B1474" s="1" t="s">
         <v>3967</v>
       </c>
-      <c r="B1474" s="1" t="s">
+      <c r="C1474" s="1" t="s">
         <v>3968</v>
-      </c>
-      <c r="C1474" s="1" t="s">
-        <v>3969</v>
       </c>
     </row>
     <row r="1475" spans="1:3">
       <c r="A1475" s="1" t="s">
-        <v>3970</v>
+        <v>3969</v>
       </c>
       <c r="B1475" s="1" t="s">
         <v>1473</v>
@@ -29081,7 +29082,7 @@
     </row>
     <row r="1476" spans="1:3">
       <c r="A1476" s="1" t="s">
-        <v>3971</v>
+        <v>3970</v>
       </c>
       <c r="B1476" s="1" t="s">
         <v>1682</v>
@@ -29092,51 +29093,51 @@
     </row>
     <row r="1477" spans="1:3">
       <c r="A1477" s="1" t="s">
+        <v>3971</v>
+      </c>
+      <c r="B1477" s="1" t="s">
         <v>3972</v>
       </c>
-      <c r="B1477" s="1" t="s">
+      <c r="C1477" s="1" t="s">
         <v>3973</v>
-      </c>
-      <c r="C1477" s="1" t="s">
-        <v>3974</v>
       </c>
     </row>
     <row r="1478" spans="1:3">
       <c r="A1478" s="1" t="s">
+        <v>3974</v>
+      </c>
+      <c r="B1478" s="1" t="s">
         <v>3975</v>
       </c>
-      <c r="B1478" s="1" t="s">
+      <c r="C1478" s="1" t="s">
         <v>3976</v>
-      </c>
-      <c r="C1478" s="1" t="s">
-        <v>3977</v>
       </c>
     </row>
     <row r="1479" spans="1:3">
       <c r="A1479" s="1" t="s">
+        <v>3977</v>
+      </c>
+      <c r="B1479" s="1" t="s">
         <v>3978</v>
       </c>
-      <c r="B1479" s="1" t="s">
+      <c r="C1479" s="1" t="s">
         <v>3979</v>
-      </c>
-      <c r="C1479" s="1" t="s">
-        <v>3980</v>
       </c>
     </row>
     <row r="1480" spans="1:3">
       <c r="A1480" s="1" t="s">
+        <v>3980</v>
+      </c>
+      <c r="B1480" s="1" t="s">
         <v>3981</v>
       </c>
-      <c r="B1480" s="1" t="s">
+      <c r="C1480" s="1" t="s">
         <v>3982</v>
-      </c>
-      <c r="C1480" s="1" t="s">
-        <v>3983</v>
       </c>
     </row>
     <row r="1481" spans="1:3">
       <c r="A1481" s="1" t="s">
-        <v>3984</v>
+        <v>3983</v>
       </c>
       <c r="B1481" s="1" t="s">
         <v>1476</v>
@@ -29147,62 +29148,62 @@
     </row>
     <row r="1482" spans="1:3">
       <c r="A1482" s="1" t="s">
-        <v>3985</v>
+        <v>3984</v>
       </c>
       <c r="B1482" s="1" t="s">
         <v>1684</v>
       </c>
       <c r="C1482" s="1" t="s">
-        <v>3986</v>
+        <v>3985</v>
       </c>
     </row>
     <row r="1483" spans="1:3">
       <c r="A1483" s="1" t="s">
+        <v>3986</v>
+      </c>
+      <c r="B1483" s="1" t="s">
         <v>3987</v>
       </c>
-      <c r="B1483" s="1" t="s">
+      <c r="C1483" s="1" t="s">
         <v>3988</v>
-      </c>
-      <c r="C1483" s="1" t="s">
-        <v>3989</v>
       </c>
     </row>
     <row r="1484" spans="1:3">
       <c r="A1484" s="1" t="s">
+        <v>3989</v>
+      </c>
+      <c r="B1484" s="1" t="s">
         <v>3990</v>
       </c>
-      <c r="B1484" s="1" t="s">
+      <c r="C1484" s="1" t="s">
         <v>3991</v>
-      </c>
-      <c r="C1484" s="1" t="s">
-        <v>3992</v>
       </c>
     </row>
     <row r="1485" spans="1:3">
       <c r="A1485" s="1" t="s">
+        <v>3992</v>
+      </c>
+      <c r="B1485" s="1" t="s">
         <v>3993</v>
       </c>
-      <c r="B1485" s="1" t="s">
+      <c r="C1485" s="1" t="s">
         <v>3994</v>
-      </c>
-      <c r="C1485" s="1" t="s">
-        <v>3995</v>
       </c>
     </row>
     <row r="1486" spans="1:3">
       <c r="A1486" s="1" t="s">
+        <v>3995</v>
+      </c>
+      <c r="B1486" s="1" t="s">
         <v>3996</v>
       </c>
-      <c r="B1486" s="1" t="s">
+      <c r="C1486" s="1" t="s">
         <v>3997</v>
-      </c>
-      <c r="C1486" s="1" t="s">
-        <v>3998</v>
       </c>
     </row>
     <row r="1487" spans="1:3">
       <c r="A1487" s="1" t="s">
-        <v>3999</v>
+        <v>3998</v>
       </c>
       <c r="B1487" s="1" t="s">
         <v>227</v>
@@ -29213,40 +29214,40 @@
     </row>
     <row r="1488" spans="1:3">
       <c r="A1488" s="1" t="s">
-        <v>4000</v>
+        <v>3999</v>
       </c>
       <c r="B1488" s="1" t="s">
         <v>187</v>
       </c>
       <c r="C1488" s="1" t="s">
-        <v>4001</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="1489" spans="1:3">
       <c r="A1489" s="1" t="s">
+        <v>4001</v>
+      </c>
+      <c r="B1489" s="1" t="s">
         <v>4002</v>
       </c>
-      <c r="B1489" s="1" t="s">
+      <c r="C1489" s="1" t="s">
         <v>4003</v>
-      </c>
-      <c r="C1489" s="1" t="s">
-        <v>4004</v>
       </c>
     </row>
     <row r="1490" spans="1:3">
       <c r="A1490" s="1" t="s">
-        <v>4005</v>
+        <v>4004</v>
       </c>
       <c r="B1490" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C1490" s="1" t="s">
-        <v>4006</v>
+        <v>4005</v>
       </c>
     </row>
     <row r="1491" spans="1:3">
       <c r="A1491" s="1" t="s">
-        <v>4007</v>
+        <v>4006</v>
       </c>
       <c r="B1491" s="1" t="s">
         <v>1235</v>
@@ -29257,7 +29258,7 @@
     </row>
     <row r="1492" spans="1:3">
       <c r="A1492" s="1" t="s">
-        <v>4008</v>
+        <v>4007</v>
       </c>
       <c r="B1492" s="1" t="s">
         <v>1485</v>
@@ -29268,43 +29269,43 @@
     </row>
     <row r="1493" spans="1:3">
       <c r="A1493" s="1" t="s">
+        <v>4008</v>
+      </c>
+      <c r="B1493" s="1" t="s">
         <v>4009</v>
       </c>
-      <c r="B1493" s="1" t="s">
+      <c r="C1493" s="1" t="s">
         <v>4010</v>
-      </c>
-      <c r="C1493" s="1" t="s">
-        <v>4011</v>
       </c>
     </row>
     <row r="1494" spans="1:3">
       <c r="A1494" s="1" t="s">
+        <v>4011</v>
+      </c>
+      <c r="B1494" s="1" t="s">
         <v>4012</v>
       </c>
-      <c r="B1494" s="1" t="s">
+      <c r="C1494" s="1" t="s">
         <v>4013</v>
-      </c>
-      <c r="C1494" s="1" t="s">
-        <v>4014</v>
       </c>
     </row>
     <row r="1495" spans="1:3">
       <c r="A1495" s="1" t="s">
+        <v>4014</v>
+      </c>
+      <c r="B1495" s="1" t="s">
         <v>4015</v>
       </c>
-      <c r="B1495" s="1" t="s">
+      <c r="C1495" s="1" t="s">
         <v>4016</v>
-      </c>
-      <c r="C1495" s="1" t="s">
-        <v>4017</v>
       </c>
     </row>
     <row r="1496" spans="1:3">
       <c r="A1496" s="1" t="s">
+        <v>4017</v>
+      </c>
+      <c r="B1496" s="1" t="s">
         <v>4018</v>
-      </c>
-      <c r="B1496" s="1" t="s">
-        <v>4019</v>
       </c>
       <c r="C1496" s="1" t="s">
         <v>237</v>
@@ -29312,7 +29313,7 @@
     </row>
     <row r="1497" spans="1:3">
       <c r="A1497" s="1" t="s">
-        <v>4020</v>
+        <v>4019</v>
       </c>
       <c r="B1497" s="1" t="s">
         <v>2050</v>
@@ -29323,95 +29324,95 @@
     </row>
     <row r="1498" spans="1:3">
       <c r="A1498" s="1" t="s">
+        <v>4020</v>
+      </c>
+      <c r="B1498" s="1" t="s">
         <v>4021</v>
       </c>
-      <c r="B1498" s="1" t="s">
+      <c r="C1498" s="1" t="s">
         <v>4022</v>
-      </c>
-      <c r="C1498" s="1" t="s">
-        <v>4023</v>
       </c>
     </row>
     <row r="1499" spans="1:3">
       <c r="A1499" s="1" t="s">
+        <v>4023</v>
+      </c>
+      <c r="B1499" s="1" t="s">
         <v>4024</v>
       </c>
-      <c r="B1499" s="1" t="s">
+      <c r="C1499" s="1" t="s">
         <v>4025</v>
-      </c>
-      <c r="C1499" s="1" t="s">
-        <v>4026</v>
       </c>
     </row>
     <row r="1500" spans="1:3">
       <c r="A1500" s="1" t="s">
+        <v>4026</v>
+      </c>
+      <c r="B1500" s="1" t="s">
         <v>4027</v>
       </c>
-      <c r="B1500" s="1" t="s">
+      <c r="C1500" s="1" t="s">
         <v>4028</v>
-      </c>
-      <c r="C1500" s="1" t="s">
-        <v>4029</v>
       </c>
     </row>
     <row r="1501" spans="1:3">
       <c r="A1501" s="1" t="s">
+        <v>4029</v>
+      </c>
+      <c r="B1501" s="1" t="s">
         <v>4030</v>
       </c>
-      <c r="B1501" s="1" t="s">
+      <c r="C1501" s="1" t="s">
         <v>4031</v>
-      </c>
-      <c r="C1501" s="1" t="s">
-        <v>4032</v>
       </c>
     </row>
     <row r="1502" spans="1:3">
       <c r="A1502" s="1" t="s">
+        <v>4032</v>
+      </c>
+      <c r="B1502" s="1" t="s">
         <v>4033</v>
       </c>
-      <c r="B1502" s="1" t="s">
+      <c r="C1502" s="1" t="s">
         <v>4034</v>
-      </c>
-      <c r="C1502" s="1" t="s">
-        <v>4035</v>
       </c>
     </row>
     <row r="1503" spans="1:3">
       <c r="A1503" s="1" t="s">
+        <v>4035</v>
+      </c>
+      <c r="B1503" s="1" t="s">
         <v>4036</v>
       </c>
-      <c r="B1503" s="1" t="s">
+      <c r="C1503" s="1" t="s">
         <v>4037</v>
-      </c>
-      <c r="C1503" s="1" t="s">
-        <v>4038</v>
       </c>
     </row>
     <row r="1504" spans="1:3">
       <c r="A1504" s="1" t="s">
+        <v>4038</v>
+      </c>
+      <c r="B1504" s="1" t="s">
         <v>4039</v>
       </c>
-      <c r="B1504" s="1" t="s">
-        <v>4040</v>
-      </c>
       <c r="C1504" s="1" t="s">
-        <v>4040</v>
+        <v>4039</v>
       </c>
     </row>
     <row r="1505" spans="1:3">
       <c r="A1505" s="1" t="s">
+        <v>4040</v>
+      </c>
+      <c r="B1505" s="1" t="s">
         <v>4041</v>
       </c>
-      <c r="B1505" s="1" t="s">
+      <c r="C1505" s="1" t="s">
         <v>4042</v>
-      </c>
-      <c r="C1505" s="1" t="s">
-        <v>4043</v>
       </c>
     </row>
     <row r="1506" spans="1:3">
       <c r="A1506" s="1" t="s">
-        <v>4044</v>
+        <v>4043</v>
       </c>
       <c r="B1506" s="1" t="s">
         <v>71</v>
@@ -29422,40 +29423,40 @@
     </row>
     <row r="1507" spans="1:3">
       <c r="A1507" s="1" t="s">
+        <v>4044</v>
+      </c>
+      <c r="B1507" s="1" t="s">
         <v>4045</v>
       </c>
-      <c r="B1507" s="1" t="s">
+      <c r="C1507" s="1" t="s">
         <v>4046</v>
-      </c>
-      <c r="C1507" s="1" t="s">
-        <v>4047</v>
       </c>
     </row>
     <row r="1508" spans="1:3">
       <c r="A1508" s="1" t="s">
+        <v>4047</v>
+      </c>
+      <c r="B1508" s="1" t="s">
         <v>4048</v>
       </c>
-      <c r="B1508" s="1" t="s">
+      <c r="C1508" s="1" t="s">
         <v>4049</v>
-      </c>
-      <c r="C1508" s="1" t="s">
-        <v>4050</v>
       </c>
     </row>
     <row r="1509" spans="1:3">
       <c r="A1509" s="1" t="s">
+        <v>4050</v>
+      </c>
+      <c r="B1509" s="1" t="s">
         <v>4051</v>
       </c>
-      <c r="B1509" s="1" t="s">
+      <c r="C1509" s="1" t="s">
         <v>4052</v>
-      </c>
-      <c r="C1509" s="1" t="s">
-        <v>4053</v>
       </c>
     </row>
     <row r="1510" spans="1:3">
       <c r="A1510" s="1" t="s">
-        <v>4054</v>
+        <v>4053</v>
       </c>
       <c r="B1510" s="1" t="s">
         <v>1263</v>
@@ -29466,7 +29467,7 @@
     </row>
     <row r="1511" spans="1:3">
       <c r="A1511" s="1" t="s">
-        <v>4055</v>
+        <v>4054</v>
       </c>
       <c r="B1511" s="1" t="s">
         <v>14</v>
@@ -29477,95 +29478,95 @@
     </row>
     <row r="1512" spans="1:3">
       <c r="A1512" s="1" t="s">
+        <v>4055</v>
+      </c>
+      <c r="B1512" s="1" t="s">
         <v>4056</v>
       </c>
-      <c r="B1512" s="1" t="s">
+      <c r="C1512" s="1" t="s">
         <v>4057</v>
-      </c>
-      <c r="C1512" s="1" t="s">
-        <v>4058</v>
       </c>
     </row>
     <row r="1513" spans="1:3">
       <c r="A1513" s="1" t="s">
-        <v>4059</v>
+        <v>4058</v>
       </c>
       <c r="B1513" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C1513" s="1" t="s">
-        <v>4060</v>
+        <v>4059</v>
       </c>
     </row>
     <row r="1514" spans="1:3">
       <c r="A1514" s="1" t="s">
+        <v>4060</v>
+      </c>
+      <c r="B1514" s="1" t="s">
         <v>4061</v>
       </c>
-      <c r="B1514" s="1" t="s">
+      <c r="C1514" s="1" t="s">
         <v>4062</v>
-      </c>
-      <c r="C1514" s="1" t="s">
-        <v>4063</v>
       </c>
     </row>
     <row r="1515" spans="1:3">
       <c r="A1515" s="1" t="s">
+        <v>4063</v>
+      </c>
+      <c r="B1515" s="1" t="s">
         <v>4064</v>
       </c>
-      <c r="B1515" s="1" t="s">
+      <c r="C1515" s="1" t="s">
         <v>4065</v>
-      </c>
-      <c r="C1515" s="1" t="s">
-        <v>4066</v>
       </c>
     </row>
     <row r="1516" spans="1:3">
       <c r="A1516" s="1" t="s">
+        <v>4066</v>
+      </c>
+      <c r="B1516" s="1" t="s">
         <v>4067</v>
       </c>
-      <c r="B1516" s="1" t="s">
+      <c r="C1516" s="1" t="s">
         <v>4068</v>
-      </c>
-      <c r="C1516" s="1" t="s">
-        <v>4069</v>
       </c>
     </row>
     <row r="1517" spans="1:3">
       <c r="A1517" s="1" t="s">
+        <v>4069</v>
+      </c>
+      <c r="B1517" s="1" t="s">
         <v>4070</v>
       </c>
-      <c r="B1517" s="1" t="s">
+      <c r="C1517" s="1" t="s">
         <v>4071</v>
-      </c>
-      <c r="C1517" s="1" t="s">
-        <v>4072</v>
       </c>
     </row>
     <row r="1518" spans="1:3">
       <c r="A1518" s="1" t="s">
+        <v>4072</v>
+      </c>
+      <c r="B1518" s="1" t="s">
         <v>4073</v>
       </c>
-      <c r="B1518" s="1" t="s">
+      <c r="C1518" s="1" t="s">
         <v>4074</v>
-      </c>
-      <c r="C1518" s="1" t="s">
-        <v>4075</v>
       </c>
     </row>
     <row r="1519" spans="1:3">
       <c r="A1519" s="1" t="s">
-        <v>4076</v>
+        <v>4075</v>
       </c>
       <c r="B1519" s="1" t="s">
         <v>1861</v>
       </c>
       <c r="C1519" s="1" t="s">
-        <v>4077</v>
+        <v>4076</v>
       </c>
     </row>
     <row r="1520" spans="1:3">
       <c r="A1520" s="1" t="s">
-        <v>4078</v>
+        <v>4077</v>
       </c>
       <c r="B1520" s="1" t="s">
         <v>1861</v>
@@ -29576,29 +29577,29 @@
     </row>
     <row r="1521" spans="1:3">
       <c r="A1521" s="1" t="s">
+        <v>4078</v>
+      </c>
+      <c r="B1521" s="1" t="s">
         <v>4079</v>
       </c>
-      <c r="B1521" s="1" t="s">
+      <c r="C1521" s="1" t="s">
         <v>4080</v>
-      </c>
-      <c r="C1521" s="1" t="s">
-        <v>4081</v>
       </c>
     </row>
     <row r="1522" spans="1:3">
       <c r="A1522" s="1" t="s">
+        <v>4081</v>
+      </c>
+      <c r="B1522" s="1" t="s">
         <v>4082</v>
       </c>
-      <c r="B1522" s="1" t="s">
+      <c r="C1522" s="1" t="s">
         <v>4083</v>
-      </c>
-      <c r="C1522" s="1" t="s">
-        <v>4084</v>
       </c>
     </row>
     <row r="1523" spans="1:3">
       <c r="A1523" s="1" t="s">
-        <v>4085</v>
+        <v>4084</v>
       </c>
       <c r="B1523" s="1" t="s">
         <v>2053</v>
@@ -29609,29 +29610,29 @@
     </row>
     <row r="1524" spans="1:3">
       <c r="A1524" s="1" t="s">
+        <v>4085</v>
+      </c>
+      <c r="B1524" s="1" t="s">
         <v>4086</v>
       </c>
-      <c r="B1524" s="1" t="s">
+      <c r="C1524" s="1" t="s">
         <v>4087</v>
-      </c>
-      <c r="C1524" s="1" t="s">
-        <v>4088</v>
       </c>
     </row>
     <row r="1525" spans="1:3">
       <c r="A1525" s="1" t="s">
+        <v>4088</v>
+      </c>
+      <c r="B1525" s="1" t="s">
         <v>4089</v>
       </c>
-      <c r="B1525" s="1" t="s">
+      <c r="C1525" s="1" t="s">
         <v>4090</v>
-      </c>
-      <c r="C1525" s="1" t="s">
-        <v>4091</v>
       </c>
     </row>
     <row r="1526" spans="1:3">
       <c r="A1526" s="1" t="s">
-        <v>4092</v>
+        <v>4091</v>
       </c>
       <c r="B1526" s="1" t="s">
         <v>1488</v>
@@ -29642,73 +29643,73 @@
     </row>
     <row r="1527" spans="1:3">
       <c r="A1527" s="1" t="s">
+        <v>4092</v>
+      </c>
+      <c r="B1527" s="1" t="s">
         <v>4093</v>
       </c>
-      <c r="B1527" s="1" t="s">
+      <c r="C1527" s="1" t="s">
         <v>4094</v>
-      </c>
-      <c r="C1527" s="1" t="s">
-        <v>4095</v>
       </c>
     </row>
     <row r="1528" spans="1:3">
       <c r="A1528" s="1" t="s">
+        <v>4095</v>
+      </c>
+      <c r="B1528" s="1" t="s">
         <v>4096</v>
       </c>
-      <c r="B1528" s="1" t="s">
+      <c r="C1528" s="1" t="s">
         <v>4097</v>
-      </c>
-      <c r="C1528" s="1" t="s">
-        <v>4098</v>
       </c>
     </row>
     <row r="1529" spans="1:3">
       <c r="A1529" s="1" t="s">
+        <v>4098</v>
+      </c>
+      <c r="B1529" s="1" t="s">
         <v>4099</v>
       </c>
-      <c r="B1529" s="1" t="s">
+      <c r="C1529" s="1" t="s">
         <v>4100</v>
-      </c>
-      <c r="C1529" s="1" t="s">
-        <v>4101</v>
       </c>
     </row>
     <row r="1530" spans="1:3">
       <c r="A1530" s="1" t="s">
+        <v>4101</v>
+      </c>
+      <c r="B1530" s="1" t="s">
         <v>4102</v>
       </c>
-      <c r="B1530" s="1" t="s">
+      <c r="C1530" s="1" t="s">
         <v>4103</v>
-      </c>
-      <c r="C1530" s="1" t="s">
-        <v>4104</v>
       </c>
     </row>
     <row r="1531" spans="1:3">
       <c r="A1531" s="1" t="s">
+        <v>4104</v>
+      </c>
+      <c r="B1531" s="1" t="s">
         <v>4105</v>
       </c>
-      <c r="B1531" s="1" t="s">
+      <c r="C1531" s="1" t="s">
         <v>4106</v>
-      </c>
-      <c r="C1531" s="1" t="s">
-        <v>4107</v>
       </c>
     </row>
     <row r="1532" spans="1:3">
       <c r="A1532" s="1" t="s">
+        <v>4107</v>
+      </c>
+      <c r="B1532" s="1" t="s">
         <v>4108</v>
       </c>
-      <c r="B1532" s="1" t="s">
+      <c r="C1532" s="1" t="s">
         <v>4109</v>
-      </c>
-      <c r="C1532" s="1" t="s">
-        <v>4110</v>
       </c>
     </row>
     <row r="1533" spans="1:3">
       <c r="A1533" s="1" t="s">
-        <v>4111</v>
+        <v>4110</v>
       </c>
       <c r="B1533" s="1" t="s">
         <v>1684</v>
@@ -29719,7 +29720,7 @@
     </row>
     <row r="1534" spans="1:3">
       <c r="A1534" s="1" t="s">
-        <v>4112</v>
+        <v>4111</v>
       </c>
       <c r="B1534" s="1" t="s">
         <v>1491</v>
@@ -29730,7 +29731,7 @@
     </row>
     <row r="1535" spans="1:3">
       <c r="A1535" s="1" t="s">
-        <v>4113</v>
+        <v>4112</v>
       </c>
       <c r="B1535" s="1" t="s">
         <v>108</v>
@@ -29741,24 +29742,24 @@
     </row>
     <row r="1536" spans="1:3">
       <c r="A1536" s="1" t="s">
-        <v>4114</v>
+        <v>4113</v>
       </c>
       <c r="B1536" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C1536" s="1" t="s">
-        <v>4115</v>
+        <v>4114</v>
       </c>
     </row>
     <row r="1537" spans="1:3">
       <c r="A1537" s="1" t="s">
+        <v>4115</v>
+      </c>
+      <c r="B1537" s="1" t="s">
         <v>4116</v>
       </c>
-      <c r="B1537" s="1" t="s">
+      <c r="C1537" s="1" t="s">
         <v>4117</v>
-      </c>
-      <c r="C1537" s="1" t="s">
-        <v>4118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Save display -> Save view
</commit_message>
<xml_diff>
--- a/Language/Resources.xlsx
+++ b/Language/Resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pasta\source\repos\NeeView\Language\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA885F5-273E-4462-BEE7-50D85C59132E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7420C6AA-A05E-4729-BD2E-EC8DF983F67E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="3525" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40260" yWindow="5565" windowWidth="26940" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="$Resources" sheetId="2" r:id="rId1"/>
@@ -12915,9 +12915,6 @@
     <t>Save as original file</t>
   </si>
   <si>
-    <t>Save display</t>
-  </si>
-  <si>
     <t>ParamCommandParameterExportImageQualityLevel</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -13025,6 +13022,10 @@
   </si>
   <si>
     <t>ControlSaveExportMode</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Save view</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -13395,7 +13396,7 @@
   <dimension ref="A1:D1572"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1544" workbookViewId="0">
-      <selection activeCell="A1572" sqref="A1572"/>
+      <selection activeCell="B1559" sqref="B1559"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -19997,7 +19998,7 @@
         <v>1668</v>
       </c>
       <c r="C599" s="1" t="s">
-        <v>4220</v>
+        <v>4219</v>
       </c>
     </row>
     <row r="600" spans="1:3">
@@ -30543,7 +30544,7 @@
         <v>4175</v>
       </c>
       <c r="B1558" s="1" t="s">
-        <v>4202</v>
+        <v>4221</v>
       </c>
       <c r="C1558" s="1" t="s">
         <v>4200</v>
@@ -30554,10 +30555,10 @@
         <v>4176</v>
       </c>
       <c r="B1559" s="1" t="s">
-        <v>4215</v>
+        <v>4214</v>
       </c>
       <c r="C1559" s="1" t="s">
-        <v>4214</v>
+        <v>4213</v>
       </c>
     </row>
     <row r="1560" spans="1:3">
@@ -30584,7 +30585,7 @@
     </row>
     <row r="1562" spans="1:3">
       <c r="A1562" s="1" t="s">
-        <v>4217</v>
+        <v>4216</v>
       </c>
       <c r="B1562" s="1" t="s">
         <v>4190</v>
@@ -30628,7 +30629,7 @@
     </row>
     <row r="1566" spans="1:3">
       <c r="A1566" s="1" t="s">
-        <v>4203</v>
+        <v>4202</v>
       </c>
       <c r="B1566" s="1" t="s">
         <v>2942</v>
@@ -30639,7 +30640,7 @@
     </row>
     <row r="1567" spans="1:3">
       <c r="A1567" s="1" t="s">
-        <v>4204</v>
+        <v>4203</v>
       </c>
       <c r="B1567" s="1" t="s">
         <v>2945</v>
@@ -30650,51 +30651,51 @@
     </row>
     <row r="1568" spans="1:3">
       <c r="A1568" s="1" t="s">
+        <v>4204</v>
+      </c>
+      <c r="B1568" s="1" t="s">
+        <v>4209</v>
+      </c>
+      <c r="C1568" s="1" t="s">
         <v>4205</v>
-      </c>
-      <c r="B1568" s="1" t="s">
-        <v>4210</v>
-      </c>
-      <c r="C1568" s="1" t="s">
-        <v>4206</v>
       </c>
     </row>
     <row r="1569" spans="1:3">
       <c r="A1569" s="1" t="s">
+        <v>4206</v>
+      </c>
+      <c r="B1569" s="1" t="s">
+        <v>4208</v>
+      </c>
+      <c r="C1569" s="1" t="s">
         <v>4207</v>
-      </c>
-      <c r="B1569" s="1" t="s">
-        <v>4209</v>
-      </c>
-      <c r="C1569" s="1" t="s">
-        <v>4208</v>
       </c>
     </row>
     <row r="1570" spans="1:3">
       <c r="A1570" s="1" t="s">
+        <v>4210</v>
+      </c>
+      <c r="B1570" s="1" t="s">
+        <v>4212</v>
+      </c>
+      <c r="C1570" s="1" t="s">
         <v>4211</v>
-      </c>
-      <c r="B1570" s="1" t="s">
-        <v>4213</v>
-      </c>
-      <c r="C1570" s="1" t="s">
-        <v>4212</v>
       </c>
     </row>
     <row r="1571" spans="1:3">
       <c r="A1571" s="1" t="s">
-        <v>4216</v>
+        <v>4215</v>
       </c>
       <c r="B1571" s="1" t="s">
-        <v>4219</v>
+        <v>4218</v>
       </c>
       <c r="C1571" s="1" t="s">
-        <v>4218</v>
+        <v>4217</v>
       </c>
     </row>
     <row r="1572" spans="1:3">
       <c r="A1572" s="1" t="s">
-        <v>4221</v>
+        <v>4220</v>
       </c>
       <c r="B1572" s="1" t="s">
         <v>4190</v>

</xml_diff>

<commit_message>
- NeeView切り替えコマンド整備 (fixed #822, #823)
</commit_message>
<xml_diff>
--- a/Language/Resources.xlsx
+++ b/Language/Resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pasta\source\repos\NeeView\Language\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9456DABC-92F9-4E8B-B41A-CD8506208413}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218229FA-C52B-4FB8-890D-691877DF5D9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14311,14 +14311,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>Next NeeView</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Prev NeeView</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>Switch to the next NeeView when multiple are started.</t>
   </si>
   <si>
@@ -14372,26 +14364,6 @@
     </rPh>
     <rPh sb="18" eb="19">
       <t>カ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>次のNeeViewに進む</t>
-    <rPh sb="0" eb="1">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>前のNeeViewに戻る</t>
-    <rPh sb="0" eb="1">
-      <t>マエ</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>モド</t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
@@ -14803,6 +14775,40 @@
   </si>
   <si>
     <t>Display according to the dpi and aspect ratio set in the image file.</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>次のNeeViewに切り替える</t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>カ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>前のNeeViewに切り替える</t>
+    <rPh sb="0" eb="1">
+      <t>マエ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>カ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Switch next NeeView</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Switch prev NeeView</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -15173,8 +15179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1677"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1266" workbookViewId="0">
-      <selection activeCell="C1363" sqref="C1363"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -16075,10 +16081,10 @@
         <v>4435</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>4438</v>
+        <v>4526</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>4447</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -16086,10 +16092,10 @@
         <v>4436</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>4438</v>
+        <v>4526</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>4447</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -16097,43 +16103,43 @@
         <v>4437</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>4440</v>
+        <v>4438</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>4441</v>
+        <v>4439</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="1" t="s">
-        <v>4442</v>
+        <v>4440</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>4439</v>
+        <v>4527</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>4448</v>
+        <v>4525</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="1" t="s">
-        <v>4443</v>
+        <v>4441</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>4439</v>
+        <v>4527</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>4448</v>
+        <v>4525</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="1" t="s">
+        <v>4442</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>4443</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>4444</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>4445</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>4446</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -16584,7 +16590,7 @@
         <v>313</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>4500</v>
+        <v>4496</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -16606,7 +16612,7 @@
         <v>318</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>4522</v>
+        <v>4518</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -18432,7 +18438,7 @@
         <v>4204</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>4483</v>
+        <v>4479</v>
       </c>
     </row>
     <row r="296" spans="1:3">
@@ -18542,7 +18548,7 @@
         <v>809</v>
       </c>
       <c r="C305" s="1" t="s">
-        <v>4471</v>
+        <v>4467</v>
       </c>
     </row>
     <row r="306" spans="1:3">
@@ -18575,7 +18581,7 @@
         <v>817</v>
       </c>
       <c r="C308" s="1" t="s">
-        <v>4474</v>
+        <v>4470</v>
       </c>
     </row>
     <row r="309" spans="1:3">
@@ -18586,7 +18592,7 @@
         <v>811</v>
       </c>
       <c r="C309" s="1" t="s">
-        <v>4485</v>
+        <v>4481</v>
       </c>
     </row>
     <row r="310" spans="1:3">
@@ -18597,7 +18603,7 @@
         <v>820</v>
       </c>
       <c r="C310" s="1" t="s">
-        <v>4472</v>
+        <v>4468</v>
       </c>
     </row>
     <row r="311" spans="1:3">
@@ -18630,7 +18636,7 @@
         <v>826</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>4475</v>
+        <v>4471</v>
       </c>
     </row>
     <row r="314" spans="1:3">
@@ -18641,7 +18647,7 @@
         <v>221</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>4486</v>
+        <v>4482</v>
       </c>
     </row>
     <row r="315" spans="1:3">
@@ -18674,7 +18680,7 @@
         <v>835</v>
       </c>
       <c r="C317" s="1" t="s">
-        <v>4493</v>
+        <v>4489</v>
       </c>
     </row>
     <row r="318" spans="1:3">
@@ -18707,7 +18713,7 @@
         <v>111</v>
       </c>
       <c r="C320" s="1" t="s">
-        <v>4494</v>
+        <v>4490</v>
       </c>
     </row>
     <row r="321" spans="1:3">
@@ -18718,7 +18724,7 @@
         <v>669</v>
       </c>
       <c r="C321" s="1" t="s">
-        <v>4495</v>
+        <v>4491</v>
       </c>
     </row>
     <row r="322" spans="1:3">
@@ -18729,7 +18735,7 @@
         <v>844</v>
       </c>
       <c r="C322" s="1" t="s">
-        <v>4476</v>
+        <v>4472</v>
       </c>
     </row>
     <row r="323" spans="1:3">
@@ -18762,7 +18768,7 @@
         <v>851</v>
       </c>
       <c r="C325" s="1" t="s">
-        <v>4484</v>
+        <v>4480</v>
       </c>
     </row>
     <row r="326" spans="1:3">
@@ -18773,7 +18779,7 @@
         <v>844</v>
       </c>
       <c r="C326" s="1" t="s">
-        <v>4487</v>
+        <v>4483</v>
       </c>
     </row>
     <row r="327" spans="1:3">
@@ -18784,7 +18790,7 @@
         <v>854</v>
       </c>
       <c r="C327" s="1" t="s">
-        <v>4477</v>
+        <v>4473</v>
       </c>
     </row>
     <row r="328" spans="1:3">
@@ -18839,7 +18845,7 @@
         <v>866</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>4478</v>
+        <v>4474</v>
       </c>
     </row>
     <row r="333" spans="1:3">
@@ -18894,7 +18900,7 @@
         <v>878</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>4479</v>
+        <v>4475</v>
       </c>
     </row>
     <row r="338" spans="1:3">
@@ -18949,7 +18955,7 @@
         <v>890</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>4480</v>
+        <v>4476</v>
       </c>
     </row>
     <row r="343" spans="1:3">
@@ -19004,7 +19010,7 @@
         <v>902</v>
       </c>
       <c r="C347" s="1" t="s">
-        <v>4523</v>
+        <v>4519</v>
       </c>
     </row>
     <row r="348" spans="1:3">
@@ -19015,7 +19021,7 @@
         <v>904</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>4497</v>
+        <v>4493</v>
       </c>
     </row>
     <row r="349" spans="1:3">
@@ -19048,7 +19054,7 @@
         <v>912</v>
       </c>
       <c r="C351" s="1" t="s">
-        <v>4496</v>
+        <v>4492</v>
       </c>
     </row>
     <row r="352" spans="1:3">
@@ -19059,7 +19065,7 @@
         <v>906</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>4497</v>
+        <v>4493</v>
       </c>
     </row>
     <row r="353" spans="1:3">
@@ -19070,7 +19076,7 @@
         <v>915</v>
       </c>
       <c r="C353" s="1" t="s">
-        <v>4499</v>
+        <v>4495</v>
       </c>
     </row>
     <row r="354" spans="1:3">
@@ -19103,7 +19109,7 @@
         <v>923</v>
       </c>
       <c r="C356" s="1" t="s">
-        <v>4498</v>
+        <v>4494</v>
       </c>
     </row>
     <row r="357" spans="1:3">
@@ -19114,7 +19120,7 @@
         <v>917</v>
       </c>
       <c r="C357" s="1" t="s">
-        <v>4499</v>
+        <v>4495</v>
       </c>
     </row>
     <row r="358" spans="1:3">
@@ -19125,7 +19131,7 @@
         <v>4292</v>
       </c>
       <c r="C358" s="1" t="s">
-        <v>4481</v>
+        <v>4477</v>
       </c>
     </row>
     <row r="359" spans="1:3">
@@ -19147,7 +19153,7 @@
         <v>930</v>
       </c>
       <c r="C360" s="1" t="s">
-        <v>4488</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="361" spans="1:3">
@@ -19180,7 +19186,7 @@
         <v>937</v>
       </c>
       <c r="C363" s="1" t="s">
-        <v>4482</v>
+        <v>4478</v>
       </c>
     </row>
     <row r="364" spans="1:3">
@@ -19213,7 +19219,7 @@
         <v>313</v>
       </c>
       <c r="C366" s="1" t="s">
-        <v>4500</v>
+        <v>4496</v>
       </c>
     </row>
     <row r="367" spans="1:3">
@@ -19224,7 +19230,7 @@
         <v>318</v>
       </c>
       <c r="C367" s="1" t="s">
-        <v>4501</v>
+        <v>4497</v>
       </c>
     </row>
     <row r="368" spans="1:3">
@@ -19664,7 +19670,7 @@
         <v>1049</v>
       </c>
       <c r="C407" s="1" t="s">
-        <v>4473</v>
+        <v>4469</v>
       </c>
     </row>
     <row r="408" spans="1:3">
@@ -19697,7 +19703,7 @@
         <v>1057</v>
       </c>
       <c r="C410" s="1" t="s">
-        <v>4502</v>
+        <v>4498</v>
       </c>
     </row>
     <row r="411" spans="1:3">
@@ -19708,7 +19714,7 @@
         <v>1051</v>
       </c>
       <c r="C411" s="1" t="s">
-        <v>4489</v>
+        <v>4485</v>
       </c>
     </row>
     <row r="412" spans="1:3">
@@ -19884,7 +19890,7 @@
         <v>1105</v>
       </c>
       <c r="C427" s="1" t="s">
-        <v>4503</v>
+        <v>4499</v>
       </c>
     </row>
     <row r="428" spans="1:3">
@@ -19939,7 +19945,7 @@
         <v>1118</v>
       </c>
       <c r="C432" s="1" t="s">
-        <v>4517</v>
+        <v>4513</v>
       </c>
     </row>
     <row r="433" spans="1:3">
@@ -19961,7 +19967,7 @@
         <v>1124</v>
       </c>
       <c r="C434" s="1" t="s">
-        <v>4519</v>
+        <v>4515</v>
       </c>
     </row>
     <row r="435" spans="1:3">
@@ -19983,7 +19989,7 @@
         <v>1130</v>
       </c>
       <c r="C436" s="1" t="s">
-        <v>4504</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="437" spans="1:3">
@@ -20038,7 +20044,7 @@
         <v>1143</v>
       </c>
       <c r="C441" s="1" t="s">
-        <v>4505</v>
+        <v>4501</v>
       </c>
     </row>
     <row r="442" spans="1:3">
@@ -20093,7 +20099,7 @@
         <v>1154</v>
       </c>
       <c r="C446" s="1" t="s">
-        <v>4506</v>
+        <v>4502</v>
       </c>
     </row>
     <row r="447" spans="1:3">
@@ -20148,7 +20154,7 @@
         <v>1165</v>
       </c>
       <c r="C451" s="1" t="s">
-        <v>4507</v>
+        <v>4503</v>
       </c>
     </row>
     <row r="452" spans="1:3">
@@ -20203,7 +20209,7 @@
         <v>1178</v>
       </c>
       <c r="C456" s="1" t="s">
-        <v>4508</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="457" spans="1:3">
@@ -20258,7 +20264,7 @@
         <v>1191</v>
       </c>
       <c r="C461" s="1" t="s">
-        <v>4509</v>
+        <v>4505</v>
       </c>
     </row>
     <row r="462" spans="1:3">
@@ -20313,7 +20319,7 @@
         <v>1204</v>
       </c>
       <c r="C466" s="1" t="s">
-        <v>4510</v>
+        <v>4506</v>
       </c>
     </row>
     <row r="467" spans="1:3">
@@ -20368,7 +20374,7 @@
         <v>1217</v>
       </c>
       <c r="C471" s="1" t="s">
-        <v>4511</v>
+        <v>4507</v>
       </c>
     </row>
     <row r="472" spans="1:3">
@@ -20423,7 +20429,7 @@
         <v>1230</v>
       </c>
       <c r="C476" s="1" t="s">
-        <v>4512</v>
+        <v>4508</v>
       </c>
     </row>
     <row r="477" spans="1:3">
@@ -20478,7 +20484,7 @@
         <v>1243</v>
       </c>
       <c r="C481" s="1" t="s">
-        <v>4513</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="482" spans="1:3">
@@ -20533,7 +20539,7 @@
         <v>1256</v>
       </c>
       <c r="C486" s="1" t="s">
-        <v>4514</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="487" spans="1:3">
@@ -20588,7 +20594,7 @@
         <v>1266</v>
       </c>
       <c r="C491" s="1" t="s">
-        <v>4515</v>
+        <v>4511</v>
       </c>
     </row>
     <row r="492" spans="1:3">
@@ -20764,7 +20770,7 @@
         <v>1312</v>
       </c>
       <c r="C507" s="1" t="s">
-        <v>4516</v>
+        <v>4512</v>
       </c>
     </row>
     <row r="508" spans="1:3">
@@ -20786,7 +20792,7 @@
         <v>1317</v>
       </c>
       <c r="C509" s="1" t="s">
-        <v>4520</v>
+        <v>4516</v>
       </c>
     </row>
     <row r="510" spans="1:3">
@@ -20808,7 +20814,7 @@
         <v>1321</v>
       </c>
       <c r="C511" s="1" t="s">
-        <v>4518</v>
+        <v>4514</v>
       </c>
     </row>
     <row r="512" spans="1:3">
@@ -20830,7 +20836,7 @@
         <v>1325</v>
       </c>
       <c r="C513" s="1" t="s">
-        <v>4521</v>
+        <v>4517</v>
       </c>
     </row>
     <row r="514" spans="1:3">
@@ -26385,7 +26391,7 @@
         <v>2585</v>
       </c>
       <c r="C1018" s="1" t="s">
-        <v>4468</v>
+        <v>4464</v>
       </c>
     </row>
     <row r="1019" spans="1:3">
@@ -26407,7 +26413,7 @@
         <v>2590</v>
       </c>
       <c r="C1020" s="1" t="s">
-        <v>4469</v>
+        <v>4465</v>
       </c>
     </row>
     <row r="1021" spans="1:3">
@@ -26759,7 +26765,7 @@
         <v>2644</v>
       </c>
       <c r="C1052" s="1" t="s">
-        <v>4470</v>
+        <v>4466</v>
       </c>
     </row>
     <row r="1053" spans="1:3">
@@ -27782,7 +27788,7 @@
         <v>2858</v>
       </c>
       <c r="C1145" s="1" t="s">
-        <v>4457</v>
+        <v>4453</v>
       </c>
     </row>
     <row r="1146" spans="1:3">
@@ -28387,7 +28393,7 @@
         <v>2972</v>
       </c>
       <c r="C1200" s="1" t="s">
-        <v>4458</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="1201" spans="1:3">
@@ -28563,7 +28569,7 @@
         <v>3004</v>
       </c>
       <c r="C1216" s="1" t="s">
-        <v>4459</v>
+        <v>4455</v>
       </c>
     </row>
     <row r="1217" spans="1:3">
@@ -28585,7 +28591,7 @@
         <v>3009</v>
       </c>
       <c r="C1218" s="1" t="s">
-        <v>4460</v>
+        <v>4456</v>
       </c>
     </row>
     <row r="1219" spans="1:3">
@@ -28629,7 +28635,7 @@
         <v>3020</v>
       </c>
       <c r="C1222" s="1" t="s">
-        <v>4461</v>
+        <v>4457</v>
       </c>
     </row>
     <row r="1223" spans="1:3">
@@ -28802,10 +28808,10 @@
         <v>3062</v>
       </c>
       <c r="B1238" s="1" t="s">
-        <v>4526</v>
+        <v>4522</v>
       </c>
       <c r="C1238" s="1" t="s">
-        <v>4525</v>
+        <v>4521</v>
       </c>
     </row>
     <row r="1239" spans="1:3">
@@ -28860,7 +28866,7 @@
         <v>4431</v>
       </c>
       <c r="C1243" s="1" t="s">
-        <v>4490</v>
+        <v>4486</v>
       </c>
     </row>
     <row r="1244" spans="1:3">
@@ -28970,7 +28976,7 @@
         <v>3090</v>
       </c>
       <c r="C1253" s="1" t="s">
-        <v>4462</v>
+        <v>4458</v>
       </c>
     </row>
     <row r="1254" spans="1:3">
@@ -29066,10 +29072,10 @@
         <v>3109</v>
       </c>
       <c r="B1262" s="1" t="s">
-        <v>4492</v>
+        <v>4488</v>
       </c>
       <c r="C1262" s="1" t="s">
-        <v>4491</v>
+        <v>4487</v>
       </c>
     </row>
     <row r="1263" spans="1:3">
@@ -29619,7 +29625,7 @@
         <v>3234</v>
       </c>
       <c r="C1312" s="1" t="s">
-        <v>4463</v>
+        <v>4459</v>
       </c>
     </row>
     <row r="1313" spans="1:3">
@@ -29806,7 +29812,7 @@
         <v>3264</v>
       </c>
       <c r="C1329" s="1" t="s">
-        <v>4453</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="1330" spans="1:3">
@@ -29916,7 +29922,7 @@
         <v>3293</v>
       </c>
       <c r="C1339" s="1" t="s">
-        <v>4454</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="1340" spans="1:3">
@@ -29982,7 +29988,7 @@
         <v>3302</v>
       </c>
       <c r="C1345" s="1" t="s">
-        <v>4464</v>
+        <v>4460</v>
       </c>
     </row>
     <row r="1346" spans="1:3">
@@ -30122,10 +30128,10 @@
         <v>3330</v>
       </c>
       <c r="B1358" s="1" t="s">
-        <v>4527</v>
+        <v>4523</v>
       </c>
       <c r="C1358" s="1" t="s">
-        <v>4524</v>
+        <v>4520</v>
       </c>
     </row>
     <row r="1359" spans="1:3">
@@ -30180,7 +30186,7 @@
         <v>3344</v>
       </c>
       <c r="C1363" s="1" t="s">
-        <v>4465</v>
+        <v>4461</v>
       </c>
     </row>
     <row r="1364" spans="1:3">
@@ -30598,7 +30604,7 @@
         <v>3444</v>
       </c>
       <c r="C1401" s="1" t="s">
-        <v>4466</v>
+        <v>4462</v>
       </c>
     </row>
     <row r="1402" spans="1:3">
@@ -30705,10 +30711,10 @@
         <v>3471</v>
       </c>
       <c r="B1411" s="1" t="s">
-        <v>4450</v>
+        <v>4446</v>
       </c>
       <c r="C1411" s="1" t="s">
-        <v>4449</v>
+        <v>4445</v>
       </c>
     </row>
     <row r="1412" spans="1:3">
@@ -30771,10 +30777,10 @@
         <v>3487</v>
       </c>
       <c r="B1417" s="1" t="s">
-        <v>4451</v>
+        <v>4447</v>
       </c>
       <c r="C1417" s="1" t="s">
-        <v>4452</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="1418" spans="1:3">
@@ -30851,7 +30857,7 @@
         <v>3507</v>
       </c>
       <c r="C1424" s="1" t="s">
-        <v>4467</v>
+        <v>4463</v>
       </c>
     </row>
     <row r="1425" spans="1:3">
@@ -31090,10 +31096,10 @@
         <v>3549</v>
       </c>
       <c r="B1446" s="1" t="s">
-        <v>4455</v>
+        <v>4451</v>
       </c>
       <c r="C1446" s="1" t="s">
-        <v>4456</v>
+        <v>4452</v>
       </c>
     </row>
     <row r="1447" spans="1:3">

</xml_diff>

<commit_message>
スクリプト：入力ダイアログ nv.ShowInputDialog() 実装 (fixed #878)
</commit_message>
<xml_diff>
--- a/Language/Resources.xlsx
+++ b/Language/Resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pasta\source\repos\NeeView\Language\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7D06B6-6724-4824-9122-1B019B3DE306}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7027D304-B777-4A7E-9961-C44DE41057A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6046" uniqueCount="5460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6058" uniqueCount="5470">
   <si>
     <t>$Key</t>
   </si>
@@ -19327,6 +19327,61 @@
   <si>
     <t>// Example: Select items that starts with "A"
 nv.Bookshelf.SelectedItems = nv.Bookshelf.Items.filter(e =&gt; e.Name.startsWith('A'))</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>入力ダイアログを表示します。</t>
+    <rPh sb="0" eb="2">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>既定のテキスト (省略可)</t>
+    <rPh sb="0" eb="2">
+      <t>キテイ</t>
+    </rPh>
+    <rPh sb="9" eb="12">
+      <t>ショウリャクカ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>入力されたテキスト。キャンセルされたときはnull</t>
+    <rPh sb="0" eb="2">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Display the input dialog.</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Default text (optional)</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Input text. Null when canceled</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>CommandHost.ShowInputDialog</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>CommandHost.ShowInputDialog.title</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>CommandHost.ShowInputDialog.text</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>CommandHost.ShowInputDialog#Returns</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -19695,10 +19750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2015"/>
+  <dimension ref="A1:D2019"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1864" workbookViewId="0">
-      <selection activeCell="B1886" sqref="B1886"/>
+    <sheetView tabSelected="1" topLeftCell="A1994" workbookViewId="0">
+      <selection activeCell="A2016" sqref="A2016:A2018"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -41879,6 +41934,50 @@
         <v>5317</v>
       </c>
     </row>
+    <row r="2016" spans="1:3">
+      <c r="A2016" s="1" t="s">
+        <v>5466</v>
+      </c>
+      <c r="B2016" s="1" t="s">
+        <v>5463</v>
+      </c>
+      <c r="C2016" s="1" t="s">
+        <v>5460</v>
+      </c>
+    </row>
+    <row r="2017" spans="1:3">
+      <c r="A2017" s="1" t="s">
+        <v>5467</v>
+      </c>
+      <c r="B2017" s="1" t="s">
+        <v>5348</v>
+      </c>
+      <c r="C2017" s="1" t="s">
+        <v>5203</v>
+      </c>
+    </row>
+    <row r="2018" spans="1:3">
+      <c r="A2018" s="1" t="s">
+        <v>5468</v>
+      </c>
+      <c r="B2018" s="1" t="s">
+        <v>5464</v>
+      </c>
+      <c r="C2018" s="1" t="s">
+        <v>5461</v>
+      </c>
+    </row>
+    <row r="2019" spans="1:3">
+      <c r="A2019" s="1" t="s">
+        <v>5469</v>
+      </c>
+      <c r="B2019" s="1" t="s">
+        <v>5465</v>
+      </c>
+      <c r="C2019" s="1" t="s">
+        <v>5462</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D1688">
     <sortCondition ref="A1109"/>

</xml_diff>

<commit_message>
- 情報パネル項目のListBox化 (fixed #1004)
</commit_message>
<xml_diff>
--- a/Language/Resources.xlsx
+++ b/Language/Resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pasta\source\repos\NeeView\Language\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE72C1C9-7722-455C-82FE-ABD67F9A0F82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291A6CCF-6581-4A82-8255-C72D24407D45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43050" yWindow="3090" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="$Resources" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6610" uniqueCount="5944">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6631" uniqueCount="5951">
   <si>
     <t>$Key</t>
   </si>
@@ -22150,34 +22150,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>Information.Image</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Information.File</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Information.Description</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Information.Origin</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Information.Camera</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Information.AdvancedPhoto</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Information.Gps</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>File</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -22733,6 +22705,62 @@
   </si>
   <si>
     <t>yyyy-MM-dd dddd H:mm</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>InformationGroup.File</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>InformationGroup.Image</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>InformationGroup.Description</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>InformationGroup.Origin</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>InformationGroup.Camera</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>InformationGroup.AdvancedPhoto</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>InformationGroup.Gps</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>xInformation.File</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>xInformation.Image</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>xInformation.Description</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>xInformation.Origin</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>xInformation.Camera</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>xInformation.AdvancedPhoto</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>xInformation.Gps</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -23121,10 +23149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2203"/>
+  <dimension ref="A1:D2210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A662" workbookViewId="0">
-      <selection activeCell="B676" sqref="B676"/>
+    <sheetView tabSelected="1" topLeftCell="A2178" workbookViewId="0">
+      <selection activeCell="F2201" sqref="F2201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -30523,7 +30551,7 @@
     </row>
     <row r="672" spans="1:3">
       <c r="A672" s="6" t="s">
-        <v>5867</v>
+        <v>5860</v>
       </c>
       <c r="B672" s="1" t="s">
         <v>1104</v>
@@ -30534,7 +30562,7 @@
     </row>
     <row r="673" spans="1:3">
       <c r="A673" s="6" t="s">
-        <v>5868</v>
+        <v>5861</v>
       </c>
       <c r="B673" s="1" t="s">
         <v>1876</v>
@@ -30545,10 +30573,10 @@
     </row>
     <row r="674" spans="1:3">
       <c r="A674" s="6" t="s">
-        <v>5942</v>
+        <v>5935</v>
       </c>
       <c r="B674" s="1" t="s">
-        <v>5943</v>
+        <v>5936</v>
       </c>
       <c r="C674" s="1" t="s">
         <v>1106</v>
@@ -30556,7 +30584,7 @@
     </row>
     <row r="675" spans="1:3">
       <c r="A675" s="6" t="s">
-        <v>5869</v>
+        <v>5862</v>
       </c>
       <c r="B675" s="1" t="s">
         <v>1875</v>
@@ -30567,7 +30595,7 @@
     </row>
     <row r="676" spans="1:3">
       <c r="A676" s="6" t="s">
-        <v>5870</v>
+        <v>5863</v>
       </c>
       <c r="B676" s="1" t="s">
         <v>1107</v>
@@ -30578,7 +30606,7 @@
     </row>
     <row r="677" spans="1:3">
       <c r="A677" s="6" t="s">
-        <v>5871</v>
+        <v>5864</v>
       </c>
       <c r="B677" s="1" t="s">
         <v>1109</v>
@@ -30589,7 +30617,7 @@
     </row>
     <row r="678" spans="1:3">
       <c r="A678" s="6" t="s">
-        <v>5872</v>
+        <v>5865</v>
       </c>
       <c r="B678" s="1" t="s">
         <v>132</v>
@@ -30600,7 +30628,7 @@
     </row>
     <row r="679" spans="1:3">
       <c r="A679" s="6" t="s">
-        <v>5873</v>
+        <v>5866</v>
       </c>
       <c r="B679" s="1" t="s">
         <v>1112</v>
@@ -30611,7 +30639,7 @@
     </row>
     <row r="680" spans="1:3">
       <c r="A680" s="6" t="s">
-        <v>5874</v>
+        <v>5867</v>
       </c>
       <c r="B680" s="1" t="s">
         <v>1113</v>
@@ -30622,7 +30650,7 @@
     </row>
     <row r="681" spans="1:3">
       <c r="A681" s="6" t="s">
-        <v>5875</v>
+        <v>5868</v>
       </c>
       <c r="B681" s="1" t="s">
         <v>6</v>
@@ -30633,7 +30661,7 @@
     </row>
     <row r="682" spans="1:3">
       <c r="A682" s="6" t="s">
-        <v>5876</v>
+        <v>5869</v>
       </c>
       <c r="B682" s="1" t="s">
         <v>1114</v>
@@ -30644,7 +30672,7 @@
     </row>
     <row r="683" spans="1:3">
       <c r="A683" s="6" t="s">
-        <v>5877</v>
+        <v>5870</v>
       </c>
       <c r="B683" s="1" t="s">
         <v>1116</v>
@@ -30655,7 +30683,7 @@
     </row>
     <row r="684" spans="1:3">
       <c r="A684" s="6" t="s">
-        <v>5878</v>
+        <v>5871</v>
       </c>
       <c r="B684" s="1" t="s">
         <v>1118</v>
@@ -30699,7 +30727,7 @@
     </row>
     <row r="688" spans="1:3">
       <c r="A688" s="6" t="s">
-        <v>5854</v>
+        <v>5847</v>
       </c>
       <c r="B688" s="1" t="s">
         <v>1451</v>
@@ -30710,7 +30738,7 @@
     </row>
     <row r="689" spans="1:3">
       <c r="A689" s="6" t="s">
-        <v>5855</v>
+        <v>5848</v>
       </c>
       <c r="B689" s="1" t="s">
         <v>1453</v>
@@ -30721,7 +30749,7 @@
     </row>
     <row r="690" spans="1:3">
       <c r="A690" s="6" t="s">
-        <v>5856</v>
+        <v>5849</v>
       </c>
       <c r="B690" s="1" t="s">
         <v>1455</v>
@@ -39777,10 +39805,10 @@
         <v>3826</v>
       </c>
       <c r="B1513" s="1" t="s">
-        <v>5939</v>
+        <v>5932</v>
       </c>
       <c r="C1513" s="1" t="s">
-        <v>5938</v>
+        <v>5931</v>
       </c>
     </row>
     <row r="1514" spans="1:3">
@@ -45505,13 +45533,13 @@
     </row>
     <row r="2034" spans="1:3">
       <c r="A2034" s="6" t="s">
-        <v>5900</v>
+        <v>5893</v>
       </c>
       <c r="B2034" s="1" t="s">
-        <v>5852</v>
+        <v>5845</v>
       </c>
       <c r="C2034" s="1" t="s">
-        <v>5853</v>
+        <v>5846</v>
       </c>
     </row>
     <row r="2035" spans="1:3">
@@ -45626,7 +45654,7 @@
     </row>
     <row r="2045" spans="1:3">
       <c r="A2045" s="6" t="s">
-        <v>5928</v>
+        <v>5921</v>
       </c>
       <c r="B2045" s="1" t="s">
         <v>1104</v>
@@ -46099,13 +46127,13 @@
     </row>
     <row r="2088" spans="1:3">
       <c r="A2088" s="6" t="s">
-        <v>5925</v>
+        <v>5918</v>
       </c>
       <c r="B2088" s="1" t="s">
-        <v>5926</v>
+        <v>5919</v>
       </c>
       <c r="C2088" s="1" t="s">
-        <v>5927</v>
+        <v>5920</v>
       </c>
     </row>
     <row r="2089" spans="1:3">
@@ -47045,54 +47073,54 @@
     </row>
     <row r="2174" spans="1:3">
       <c r="A2174" s="6" t="s">
-        <v>5831</v>
+        <v>5944</v>
       </c>
       <c r="B2174" s="1" t="s">
+        <v>5830</v>
+      </c>
+      <c r="C2174" s="1" t="s">
         <v>5837</v>
-      </c>
-      <c r="C2174" s="1" t="s">
-        <v>5844</v>
       </c>
     </row>
     <row r="2175" spans="1:3">
       <c r="A2175" s="6" t="s">
-        <v>5830</v>
+        <v>5945</v>
       </c>
       <c r="B2175" s="1" t="s">
+        <v>5831</v>
+      </c>
+      <c r="C2175" s="1" t="s">
         <v>5838</v>
-      </c>
-      <c r="C2175" s="1" t="s">
-        <v>5845</v>
       </c>
     </row>
     <row r="2176" spans="1:3">
       <c r="A2176" s="6" t="s">
+        <v>5946</v>
+      </c>
+      <c r="B2176" s="1" t="s">
         <v>5832</v>
       </c>
-      <c r="B2176" s="1" t="s">
+      <c r="C2176" s="1" t="s">
         <v>5839</v>
-      </c>
-      <c r="C2176" s="1" t="s">
-        <v>5846</v>
       </c>
     </row>
     <row r="2177" spans="1:3">
       <c r="A2177" s="6" t="s">
+        <v>5947</v>
+      </c>
+      <c r="B2177" s="1" t="s">
         <v>5833</v>
       </c>
-      <c r="B2177" s="1" t="s">
+      <c r="C2177" s="1" t="s">
         <v>5840</v>
-      </c>
-      <c r="C2177" s="1" t="s">
-        <v>5847</v>
       </c>
     </row>
     <row r="2178" spans="1:3">
       <c r="A2178" s="6" t="s">
+        <v>5948</v>
+      </c>
+      <c r="B2178" s="1" t="s">
         <v>5834</v>
-      </c>
-      <c r="B2178" s="1" t="s">
-        <v>5841</v>
       </c>
       <c r="C2178" s="1" t="s">
         <v>5575</v>
@@ -47100,277 +47128,354 @@
     </row>
     <row r="2179" spans="1:3">
       <c r="A2179" s="6" t="s">
-        <v>5835</v>
+        <v>5949</v>
       </c>
       <c r="B2179" s="1" t="s">
-        <v>5843</v>
+        <v>5836</v>
       </c>
       <c r="C2179" s="1" t="s">
-        <v>5848</v>
+        <v>5841</v>
       </c>
     </row>
     <row r="2180" spans="1:3">
       <c r="A2180" s="6" t="s">
-        <v>5836</v>
+        <v>5950</v>
       </c>
       <c r="B2180" s="1" t="s">
-        <v>5842</v>
+        <v>5835</v>
       </c>
       <c r="C2180" s="1" t="s">
-        <v>5842</v>
+        <v>5835</v>
       </c>
     </row>
     <row r="2181" spans="1:3">
       <c r="A2181" s="6" t="s">
-        <v>5849</v>
+        <v>5842</v>
       </c>
       <c r="B2181" s="1" t="s">
-        <v>5850</v>
+        <v>5843</v>
       </c>
       <c r="C2181" s="1" t="s">
-        <v>5851</v>
+        <v>5844</v>
       </c>
     </row>
     <row r="2182" spans="1:3">
       <c r="A2182" s="6" t="s">
-        <v>5857</v>
+        <v>5850</v>
       </c>
       <c r="B2182" s="1" t="s">
-        <v>5862</v>
+        <v>5855</v>
       </c>
       <c r="C2182" s="1" t="s">
-        <v>5861</v>
+        <v>5854</v>
       </c>
     </row>
     <row r="2183" spans="1:3">
       <c r="A2183" s="6" t="s">
+        <v>5851</v>
+      </c>
+      <c r="B2183" s="1" t="s">
+        <v>5859</v>
+      </c>
+      <c r="C2183" s="1" t="s">
         <v>5858</v>
-      </c>
-      <c r="B2183" s="1" t="s">
-        <v>5866</v>
-      </c>
-      <c r="C2183" s="1" t="s">
-        <v>5865</v>
       </c>
     </row>
     <row r="2184" spans="1:3">
       <c r="A2184" s="6" t="s">
-        <v>5859</v>
+        <v>5852</v>
       </c>
       <c r="B2184" s="1" t="s">
-        <v>5864</v>
+        <v>5857</v>
       </c>
       <c r="C2184" s="1" t="s">
-        <v>5863</v>
+        <v>5856</v>
       </c>
     </row>
     <row r="2185" spans="1:3">
       <c r="A2185" s="6" t="s">
-        <v>5860</v>
+        <v>5853</v>
       </c>
       <c r="B2185" s="1" t="s">
-        <v>5940</v>
+        <v>5933</v>
       </c>
       <c r="C2185" s="1" t="s">
-        <v>5941</v>
+        <v>5934</v>
       </c>
     </row>
     <row r="2186" spans="1:3">
       <c r="A2186" s="6" t="s">
+        <v>5872</v>
+      </c>
+      <c r="B2186" s="1" t="s">
+        <v>5886</v>
+      </c>
+      <c r="C2186" s="1" t="s">
         <v>5879</v>
-      </c>
-      <c r="B2186" s="1" t="s">
-        <v>5893</v>
-      </c>
-      <c r="C2186" s="1" t="s">
-        <v>5886</v>
       </c>
     </row>
     <row r="2187" spans="1:3">
       <c r="A2187" s="6" t="s">
+        <v>5873</v>
+      </c>
+      <c r="B2187" s="1" t="s">
+        <v>5887</v>
+      </c>
+      <c r="C2187" s="1" t="s">
         <v>5880</v>
-      </c>
-      <c r="B2187" s="1" t="s">
-        <v>5894</v>
-      </c>
-      <c r="C2187" s="1" t="s">
-        <v>5887</v>
       </c>
     </row>
     <row r="2188" spans="1:3">
       <c r="A2188" s="6" t="s">
-        <v>5881</v>
+        <v>5874</v>
       </c>
       <c r="B2188" s="1" t="s">
-        <v>5895</v>
+        <v>5888</v>
       </c>
       <c r="C2188" s="1" t="s">
-        <v>5889</v>
+        <v>5882</v>
       </c>
     </row>
     <row r="2189" spans="1:3">
       <c r="A2189" s="6" t="s">
-        <v>5882</v>
+        <v>5875</v>
       </c>
       <c r="B2189" s="1" t="s">
-        <v>5896</v>
+        <v>5889</v>
       </c>
       <c r="C2189" s="1" t="s">
-        <v>5888</v>
+        <v>5881</v>
       </c>
     </row>
     <row r="2190" spans="1:3">
       <c r="A2190" s="6" t="s">
+        <v>5876</v>
+      </c>
+      <c r="B2190" s="1" t="s">
+        <v>5890</v>
+      </c>
+      <c r="C2190" s="1" t="s">
         <v>5883</v>
-      </c>
-      <c r="B2190" s="1" t="s">
-        <v>5897</v>
-      </c>
-      <c r="C2190" s="1" t="s">
-        <v>5890</v>
       </c>
     </row>
     <row r="2191" spans="1:3">
       <c r="A2191" s="6" t="s">
+        <v>5877</v>
+      </c>
+      <c r="B2191" s="1" t="s">
+        <v>5891</v>
+      </c>
+      <c r="C2191" s="1" t="s">
         <v>5884</v>
-      </c>
-      <c r="B2191" s="1" t="s">
-        <v>5898</v>
-      </c>
-      <c r="C2191" s="1" t="s">
-        <v>5891</v>
       </c>
     </row>
     <row r="2192" spans="1:3">
       <c r="A2192" s="6" t="s">
+        <v>5878</v>
+      </c>
+      <c r="B2192" s="1" t="s">
+        <v>5892</v>
+      </c>
+      <c r="C2192" s="1" t="s">
         <v>5885</v>
-      </c>
-      <c r="B2192" s="1" t="s">
-        <v>5899</v>
-      </c>
-      <c r="C2192" s="1" t="s">
-        <v>5892</v>
       </c>
     </row>
     <row r="2193" spans="1:3">
       <c r="A2193" s="6" t="s">
-        <v>5901</v>
+        <v>5894</v>
       </c>
       <c r="B2193" s="1" t="s">
-        <v>5909</v>
+        <v>5902</v>
       </c>
       <c r="C2193" s="1" t="s">
-        <v>5910</v>
+        <v>5903</v>
       </c>
     </row>
     <row r="2194" spans="1:3">
       <c r="A2194" s="6" t="s">
-        <v>5902</v>
+        <v>5895</v>
       </c>
       <c r="B2194" s="1" t="s">
+        <v>5904</v>
+      </c>
+      <c r="C2194" s="1" t="s">
         <v>5911</v>
-      </c>
-      <c r="C2194" s="1" t="s">
-        <v>5918</v>
       </c>
     </row>
     <row r="2195" spans="1:3">
       <c r="A2195" s="6" t="s">
-        <v>5903</v>
+        <v>5896</v>
       </c>
       <c r="B2195" s="1" t="s">
-        <v>5917</v>
+        <v>5910</v>
       </c>
       <c r="C2195" s="1" t="s">
-        <v>5919</v>
+        <v>5912</v>
       </c>
     </row>
     <row r="2196" spans="1:3">
       <c r="A2196" s="6" t="s">
-        <v>5904</v>
+        <v>5897</v>
       </c>
       <c r="B2196" s="1" t="s">
-        <v>5912</v>
+        <v>5905</v>
       </c>
       <c r="C2196" s="1" t="s">
-        <v>5920</v>
+        <v>5913</v>
       </c>
     </row>
     <row r="2197" spans="1:3">
       <c r="A2197" s="6" t="s">
-        <v>5905</v>
+        <v>5898</v>
       </c>
       <c r="B2197" s="1" t="s">
-        <v>5913</v>
+        <v>5906</v>
       </c>
       <c r="C2197" s="1" t="s">
-        <v>5921</v>
+        <v>5914</v>
       </c>
     </row>
     <row r="2198" spans="1:3">
       <c r="A2198" s="6" t="s">
-        <v>5906</v>
+        <v>5899</v>
       </c>
       <c r="B2198" s="1" t="s">
+        <v>5908</v>
+      </c>
+      <c r="C2198" s="1" t="s">
         <v>5915</v>
-      </c>
-      <c r="C2198" s="1" t="s">
-        <v>5922</v>
       </c>
     </row>
     <row r="2199" spans="1:3">
       <c r="A2199" s="6" t="s">
+        <v>5900</v>
+      </c>
+      <c r="B2199" s="1" t="s">
         <v>5907</v>
       </c>
-      <c r="B2199" s="1" t="s">
-        <v>5914</v>
-      </c>
       <c r="C2199" s="1" t="s">
-        <v>5923</v>
+        <v>5916</v>
       </c>
     </row>
     <row r="2200" spans="1:3">
       <c r="A2200" s="6" t="s">
-        <v>5908</v>
+        <v>5901</v>
       </c>
       <c r="B2200" s="1" t="s">
-        <v>5916</v>
+        <v>5909</v>
       </c>
       <c r="C2200" s="1" t="s">
-        <v>5924</v>
+        <v>5917</v>
       </c>
     </row>
     <row r="2201" spans="1:3">
       <c r="A2201" s="6" t="s">
+        <v>5922</v>
+      </c>
+      <c r="B2201" s="1" t="s">
         <v>5929</v>
       </c>
-      <c r="B2201" s="1" t="s">
-        <v>5936</v>
-      </c>
       <c r="C2201" s="1" t="s">
-        <v>5932</v>
+        <v>5925</v>
       </c>
     </row>
     <row r="2202" spans="1:3">
       <c r="A2202" s="6" t="s">
+        <v>5923</v>
+      </c>
+      <c r="B2202" s="1" t="s">
         <v>5930</v>
       </c>
-      <c r="B2202" s="1" t="s">
-        <v>5937</v>
-      </c>
       <c r="C2202" s="1" t="s">
-        <v>5931</v>
+        <v>5924</v>
       </c>
     </row>
     <row r="2203" spans="1:3">
       <c r="A2203" s="6" t="s">
-        <v>5933</v>
+        <v>5926</v>
       </c>
       <c r="B2203" s="1" t="s">
-        <v>5935</v>
+        <v>5928</v>
       </c>
       <c r="C2203" s="1" t="s">
-        <v>5934</v>
+        <v>5927</v>
+      </c>
+    </row>
+    <row r="2204" spans="1:3">
+      <c r="A2204" s="6" t="s">
+        <v>5937</v>
+      </c>
+      <c r="B2204" s="1" t="s">
+        <v>5830</v>
+      </c>
+      <c r="C2204" s="1" t="s">
+        <v>5837</v>
+      </c>
+    </row>
+    <row r="2205" spans="1:3">
+      <c r="A2205" s="6" t="s">
+        <v>5938</v>
+      </c>
+      <c r="B2205" s="1" t="s">
+        <v>5831</v>
+      </c>
+      <c r="C2205" s="1" t="s">
+        <v>5838</v>
+      </c>
+    </row>
+    <row r="2206" spans="1:3">
+      <c r="A2206" s="6" t="s">
+        <v>5939</v>
+      </c>
+      <c r="B2206" s="1" t="s">
+        <v>5832</v>
+      </c>
+      <c r="C2206" s="1" t="s">
+        <v>5839</v>
+      </c>
+    </row>
+    <row r="2207" spans="1:3">
+      <c r="A2207" s="6" t="s">
+        <v>5940</v>
+      </c>
+      <c r="B2207" s="1" t="s">
+        <v>5833</v>
+      </c>
+      <c r="C2207" s="1" t="s">
+        <v>5840</v>
+      </c>
+    </row>
+    <row r="2208" spans="1:3">
+      <c r="A2208" s="6" t="s">
+        <v>5941</v>
+      </c>
+      <c r="B2208" s="1" t="s">
+        <v>5834</v>
+      </c>
+      <c r="C2208" s="1" t="s">
+        <v>5575</v>
+      </c>
+    </row>
+    <row r="2209" spans="1:3">
+      <c r="A2209" s="6" t="s">
+        <v>5942</v>
+      </c>
+      <c r="B2209" s="1" t="s">
+        <v>5836</v>
+      </c>
+      <c r="C2209" s="1" t="s">
+        <v>5841</v>
+      </c>
+    </row>
+    <row r="2210" spans="1:3">
+      <c r="A2210" s="6" t="s">
+        <v>5943</v>
+      </c>
+      <c r="B2210" s="1" t="s">
+        <v>5835</v>
+      </c>
+      <c r="C2210" s="1" t="s">
+        <v>5835</v>
       </c>
     </row>
   </sheetData>

</xml_diff>